<commit_message>
Fixed bug 13.d: Site notification must be admin
</commit_message>
<xml_diff>
--- a/_document/Bug Collectios-huy.xlsx
+++ b/_document/Bug Collectios-huy.xlsx
@@ -839,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BQ96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2643,11 +2643,23 @@
       <c r="B41" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="C41" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="42" spans="1:69">
       <c r="A42" s="14"/>
       <c r="B42" s="15" t="s">
         <v>42</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="E42" s="12"/>
       <c r="F42" s="12"/>
@@ -2720,7 +2732,7 @@
         <v>13</v>
       </c>
       <c r="C43" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D43" t="s">
         <v>33</v>
@@ -2796,12 +2808,8 @@
       <c r="B44" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C44" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D44" s="14" t="s">
-        <v>33</v>
-      </c>
+      <c r="C44"/>
+      <c r="D44"/>
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
       <c r="G44" s="12"/>
@@ -2873,12 +2881,11 @@
         <v>15</v>
       </c>
       <c r="C45" t="s">
-        <v>34</v>
-      </c>
-      <c r="D45" t="s">
-        <v>33</v>
-      </c>
-      <c r="E45" s="12"/>
+        <v>32</v>
+      </c>
+      <c r="E45" s="26" t="s">
+        <v>46</v>
+      </c>
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
       <c r="H45" s="12"/>
@@ -2947,6 +2954,9 @@
     <row r="46" spans="1:69">
       <c r="B46" s="3" t="s">
         <v>43</v>
+      </c>
+      <c r="C46" t="s">
+        <v>32</v>
       </c>
       <c r="D46" t="s">
         <v>33</v>
@@ -3019,9 +3029,6 @@
     </row>
     <row r="47" spans="1:69">
       <c r="B47" s="3"/>
-      <c r="C47" t="s">
-        <v>32</v>
-      </c>
       <c r="D47" t="s">
         <v>33</v>
       </c>
@@ -3093,12 +3100,6 @@
     </row>
     <row r="48" spans="1:69">
       <c r="B48" s="2"/>
-      <c r="C48" t="s">
-        <v>32</v>
-      </c>
-      <c r="D48" t="s">
-        <v>33</v>
-      </c>
       <c r="E48" s="12"/>
       <c r="F48" s="12"/>
       <c r="G48" s="12"/>

</xml_diff>

<commit_message>
Add lang for profile Remove email field from editing from
</commit_message>
<xml_diff>
--- a/_document/Bug Collectios-huy.xlsx
+++ b/_document/Bug Collectios-huy.xlsx
@@ -361,7 +361,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -423,6 +423,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -845,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BQ96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1479,7 +1480,7 @@
       <c r="BQ13" s="12"/>
     </row>
     <row r="14" spans="1:69">
-      <c r="A14" s="11">
+      <c r="A14" s="27">
         <v>9.1999999999999993</v>
       </c>
       <c r="B14" s="2" t="s">

</xml_diff>

<commit_message>
Fix CSS cho event_calendar, Chỉnh sửa profile, và tối ưu hóa profile.
</commit_message>
<xml_diff>
--- a/_document/Bug Collectios-huy.xlsx
+++ b/_document/Bug Collectios-huy.xlsx
@@ -776,7 +776,7 @@
   <dimension ref="A1:BQ75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4016,9 +4016,7 @@
       <c r="BQ53" s="10"/>
     </row>
     <row r="54" spans="2:69">
-      <c r="B54" s="6" t="s">
-        <v>16</v>
-      </c>
+      <c r="B54" s="6"/>
       <c r="E54" s="22"/>
       <c r="F54" s="10"/>
       <c r="G54" s="10"/>
@@ -4086,7 +4084,9 @@
       <c r="BQ54" s="10"/>
     </row>
     <row r="55" spans="2:69">
-      <c r="B55" s="6"/>
+      <c r="B55" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="E55" s="22"/>
       <c r="F55" s="10"/>
       <c r="G55" s="10"/>

</xml_diff>